<commit_message>
Refactor : BaseAbility 구조변경
</commit_message>
<xml_diff>
--- a/DesignData/Excel_Masters/WeaponStats_Master.xlsx
+++ b/DesignData/Excel_Masters/WeaponStats_Master.xlsx
@@ -14,14 +14,13 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Rarity" sheetId="3" r:id="rId2"/>
-    <sheet name="Tags" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>---</t>
   </si>
@@ -45,29 +44,6 @@
   </si>
   <si>
     <t>SetID</t>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Melee.Sword</t>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Melee.Sword</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Melee.GreatSword</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Melee.Dagger</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Range.Bow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item.Type.Weapon.Range.Staff</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>AttackPower</t>
@@ -75,10 +51,6 @@
   </si>
   <si>
     <t>AttackSpeed</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WeaponTag</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1046,120 +1018,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.125" customWidth="1"/>
-    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.5</v>
-      </c>
-      <c r="F2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0.2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="9">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류" error="음수(-)는 입력할 수 없습니다. 0 이상의 숫자를 입력해주세요." sqref="C2:C1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류" error="음수(-)는 입력할 수 없습니다. 0 이상의 숫자를 입력해주세요." sqref="B2:B1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="단위 확인 (Cooldown)" error="쿨타임은 0보다 작을 수 없습니다._x000a__x000a_※ 단위: 초 (Seconds)_x000a_- 1분 = '60' 입력_x000a_- 0.5초 = '0.5' 입력_x000a_- 쿨타임 없음 = '0' 입력_x000a__x000a_밀리초(ms) 단위가 아닙니다! 다시 확인해주세요." sqref="H2:H1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="단위 확인 (Cooldown)" error="쿨타임은 0보다 작을 수 없습니다._x000a__x000a_※ 단위: 초 (Seconds)_x000a_- 1분 = '60' 입력_x000a_- 0.5초 = '0.5' 입력_x000a_- 쿨타임 없음 = '0' 입력_x000a__x000a_밀리초(ms) 단위가 아닙니다! 다시 확인해주세요." sqref="G2:G1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="확률은 0.0 ~ 1.0 사이의 소수점만 가능합니다. (예: 15% -&gt; 0.15)" sqref="E2:E1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="확률은 0.0 ~ 1.0 사이의 소수점만 가능합니다. (예: 15% -&gt; 0.15)" sqref="D2:D1048576">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="CritDamage(치명타 배율)는 최소 1.0 이상이어야 합니다." sqref="F2:F1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="CritDamage(치명타 배율)는 최소 1.0 이상이어야 합니다." sqref="E2:E1048576">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류" error="음수(-)는 입력할 수 없습니다. 0 이상의 숫자를 입력해주세요." sqref="D2:D1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류" error="음수(-)는 입력할 수 없습니다. 0 이상의 숫자를 입력해주세요." sqref="C2:C1048576">
       <formula1>0.1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="사거리는 0보다 작을 수 없습니다._x000a__x000a_※ 중요: 언리얼 단위(cm) 기준입니다!_x000a_(미터법 입력 금지)_x000a__x000a_[올바른 예시]_x000a_- 1m 사거리 = '100' 입력_x000a_- 1.5m 사거리 = '150' 입력_x000a_- 5m 사거리 = '500' 입력_x000a__x000a_'1.5'라고 적으면 1.5cm가 됩니다! 다시 확인해주세요." sqref="G2:G1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="범위 오류" error="사거리는 0보다 작을 수 없습니다._x000a__x000a_※ 중요: 언리얼 단위(cm) 기준입니다!_x000a_(미터법 입력 금지)_x000a__x000a_[올바른 예시]_x000a_- 1m 사거리 = '100' 입력_x000a_- 1.5m 사거리 = '150' 입력_x000a_- 5m 사거리 = '500' 입력_x000a__x000a_'1.5'라고 적으면 1.5cm가 됩니다! 다시 확인해주세요." sqref="F2:F1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="글자 수 초과 (DisplayName)" error="아이템 이름이 너무 깁니다! (최대 20자)_x000a__x000a_UI 텍스트 박스를 넘어갈 위험이 있습니다._x000a_더 짧게 줄이거나, 줄바꿈이 필요한지 확인해주세요." sqref="I2:I1048576">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="글자 수 초과 (DisplayName)" error="아이템 이름이 너무 깁니다! (최대 20자)_x000a__x000a_UI 텍스트 박스를 넘어갈 위험이 있습니다._x000a_더 짧게 줄이거나, 줄바꿈이 필요한지 확인해주세요." sqref="H2:H1048576">
       <formula1>20</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="설명 길이 확인" error="설명이 너무 깁니다. (100자 제한)_x000a__x000a_※ 팁:_x000a_줄바꿈이 필요하면 [Alt + Enter]를 사용하세요._x000a_너무 긴 설명은 툴팁 가독성을 해칩니다." sqref="J2:J1048576">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="설명 길이 확인" error="설명이 너무 깁니다. (100자 제한)_x000a__x000a_※ 팁:_x000a_줄바꿈이 필요하면 [Alt + Enter]를 사용하세요._x000a_너무 긴 설명은 툴팁 가독성을 해칩니다." sqref="I2:I1048576">
       <formula1>100</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="중복된 ID (RowName Error)" error="이미 존재하는 ID입니다!_x000a__x000a_RowName(행 이름)은 고유해야 합니다._x000a_(같은 이름을 두 번 쓸 수 없습니다.)_x000a__x000a_다른 이름을 입력해주세요." sqref="A1:A1048576">
@@ -1169,24 +1134,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Tags!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:B1048576 B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="선택 오류" error="목록에 없는 값입니다! 드롭다운(▼)을 눌러서 선택해주세요.">
-          <x14:formula1>
-            <xm:f>Tags!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="목록 선택 (Rarity)" error="목록에 없는 희귀도입니다._x000a__x000a_직접 타이핑하지 마시고, 드롭다운(▼) 버튼을 눌러 목록에서 선택해주세요._x000a_(오타 발생 시 게임 내 테두리 색상이 깨집니다.)">
           <x14:formula1>
             <xm:f>Rarity!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1206,68 +1159,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>